<commit_message>
Chinh sua do an
</commit_message>
<xml_diff>
--- a/Kehoachdoan.xlsx
+++ b/Kehoachdoan.xlsx
@@ -266,13 +266,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -280,12 +280,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -310,6 +304,12 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -327,15 +327,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:I32" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A2:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="STT" dataDxfId="0"/>
-    <tableColumn id="2" name="Các thao tác" dataDxfId="1"/>
-    <tableColumn id="3" name="Phần việc cụ thể" dataDxfId="8"/>
-    <tableColumn id="4" name="Phước Toàn" dataDxfId="7"/>
-    <tableColumn id="5" name="Ngoc Nhi" dataDxfId="6"/>
-    <tableColumn id="6" name="Ngày bắt đầu(dự tính)" dataDxfId="5"/>
-    <tableColumn id="7" name="Ngày hoàn thành(dự tính)" dataDxfId="4"/>
-    <tableColumn id="8" name="Ngày bắt đầu(thực)" dataDxfId="3"/>
-    <tableColumn id="9" name="Ngày hoàn thành(thực)" dataDxfId="2"/>
+    <tableColumn id="1" name="STT" dataDxfId="8"/>
+    <tableColumn id="2" name="Các thao tác" dataDxfId="7"/>
+    <tableColumn id="3" name="Phần việc cụ thể" dataDxfId="6"/>
+    <tableColumn id="4" name="Phước Toàn" dataDxfId="5"/>
+    <tableColumn id="5" name="Ngoc Nhi" dataDxfId="4"/>
+    <tableColumn id="6" name="Ngày bắt đầu(dự tính)" dataDxfId="3"/>
+    <tableColumn id="7" name="Ngày hoàn thành(dự tính)" dataDxfId="2"/>
+    <tableColumn id="8" name="Ngày bắt đầu(thực)" dataDxfId="1"/>
+    <tableColumn id="9" name="Ngày hoàn thành(thực)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -606,7 +606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -624,17 +624,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -666,7 +666,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -689,7 +689,7 @@
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="5"/>
       <c r="C4" s="4" t="s">
         <v>12</v>

</xml_diff>